<commit_message>
Agregados 3 casos de prueba
</commit_message>
<xml_diff>
--- a/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-4.xlsx
+++ b/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-4.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Casos de Prueba'!$A$11:$M$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Prueba'!$A$1:$M$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Prueba'!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t xml:space="preserve">RESULTADO OBTENIDO </t>
   </si>
@@ -243,10 +243,121 @@
     <t>Gonzalo López</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>N° Caso de Uso</t>
   </si>
   <si>
     <t xml:space="preserve">Personal médico, Médico </t>
+  </si>
+  <si>
+    <t>CUS-15</t>
+  </si>
+  <si>
+    <t>Abrir caja</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>Ingresar valores negativos y alfabéticos</t>
+  </si>
+  <si>
+    <t>Valores inválidos</t>
+  </si>
+  <si>
+    <t>Valores no permitidos en el campo</t>
+  </si>
+  <si>
+    <t>No se permite ingreso de caracteres alfabéticos ni especiales. Se pueden pegar desde fuentes externas pero la aplicación sigue sin permitir su ingreso</t>
+  </si>
+  <si>
+    <t>CUS-16</t>
+  </si>
+  <si>
+    <t>Cerrar caja</t>
+  </si>
+  <si>
+    <t>Cerrar la caja para terminar transacciones diarias</t>
+  </si>
+  <si>
+    <t>Abrir la caja para permitir transacciones diarias</t>
+  </si>
+  <si>
+    <t>Abrir 2 cajas en un día</t>
+  </si>
+  <si>
+    <t>Volver a la opción de abrir caja</t>
+  </si>
+  <si>
+    <t>Botón bloqueado</t>
+  </si>
+  <si>
+    <t>No permitir abrir otra caja</t>
+  </si>
+  <si>
+    <t>CUS-2</t>
+  </si>
+  <si>
+    <t>Agendar atención</t>
+  </si>
+  <si>
+    <t>Registrar una atención para un paciente</t>
+  </si>
+  <si>
+    <t>Paciente no existente</t>
+  </si>
+  <si>
+    <t>Fecha pasada</t>
+  </si>
+  <si>
+    <t>Día sin horas disponibles</t>
+  </si>
+  <si>
+    <t>Ingresar valor de dinero en caja</t>
+  </si>
+  <si>
+    <t>Caja abierta correctamente</t>
+  </si>
+  <si>
+    <t>La caja se abre sin problemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrar caja </t>
+  </si>
+  <si>
+    <t>Cerrar caja correctamente</t>
+  </si>
+  <si>
+    <t>La caja se cierra sin problemas</t>
+  </si>
+  <si>
+    <t>Ingresar valores correctos para agendar</t>
+  </si>
+  <si>
+    <t>Atención agendada correctamente</t>
+  </si>
+  <si>
+    <t>Ingresar Rut de paciente no existente</t>
+  </si>
+  <si>
+    <t>Paciente no encontrado</t>
+  </si>
+  <si>
+    <t>La atención se registra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se muestra un mensaje de error y no permite el agendamiento </t>
+  </si>
+  <si>
+    <t>Poner una fecha anterior a hoy</t>
+  </si>
+  <si>
+    <t>Atención agendada no permitida</t>
+  </si>
+  <si>
+    <t>Agendar en un día domingo</t>
   </si>
 </sst>
 </file>
@@ -462,36 +573,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -518,19 +599,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -833,11 +901,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -899,36 +1006,40 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -936,18 +1047,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -955,7 +1062,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -963,18 +1078,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -982,7 +1089,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -990,11 +1109,73 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1002,97 +1183,23 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1113,27 +1220,27 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1141,29 +1248,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1179,19 +1286,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1199,65 +1302,55 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1265,69 +1358,103 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1870,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4759"/>
+  <dimension ref="A1:O4761"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:M22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="10.5" x14ac:dyDescent="0.2"/>
@@ -1908,35 +2035,35 @@
     </row>
     <row r="2" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
@@ -1948,149 +2075,149 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="108" t="s">
+      <c r="D5" s="108"/>
+      <c r="E5" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="109"/>
-      <c r="M5" s="111"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="105"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="112" t="s">
+      <c r="D6" s="107"/>
+      <c r="E6" s="106" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="106" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="107"/>
+      <c r="E7" s="106" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="110"/>
+    </row>
+    <row r="8" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C8" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="107"/>
+      <c r="E8" s="106" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="110"/>
+    </row>
+    <row r="9" spans="1:15" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="120" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="121"/>
+      <c r="E9" s="99">
+        <v>42702</v>
+      </c>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="117"/>
+    </row>
+    <row r="10" spans="1:15" s="8" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+    </row>
+    <row r="11" spans="1:15" s="10" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="116"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="112" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="112" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="116"/>
-    </row>
-    <row r="8" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C8" s="112" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="112" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115"/>
-      <c r="M8" s="116"/>
-    </row>
-    <row r="9" spans="1:15" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="126" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="127"/>
-      <c r="E9" s="105">
-        <v>42702</v>
-      </c>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="122"/>
-      <c r="L9" s="122"/>
-      <c r="M9" s="123"/>
-    </row>
-    <row r="10" spans="1:15" s="8" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="124"/>
-      <c r="D10" s="124"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="125"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="125"/>
-      <c r="L10" s="125"/>
-      <c r="M10" s="125"/>
-    </row>
-    <row r="11" spans="1:15" s="10" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="120" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="132" t="s">
+      <c r="E11" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="120" t="s">
+      <c r="F11" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="120" t="s">
+      <c r="G11" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="120" t="s">
+      <c r="H11" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="129" t="s">
+      <c r="I11" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="130"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="130"/>
-      <c r="M11" s="131"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="125"/>
     </row>
     <row r="12" spans="1:15" s="10" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="135"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="128"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
       <c r="I12" s="11" t="s">
         <v>2</v>
       </c>
@@ -2107,140 +2234,320 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="93"/>
-    </row>
-    <row r="14" spans="1:15" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="98"/>
-    </row>
-    <row r="15" spans="1:15" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="98"/>
-    </row>
-    <row r="16" spans="1:15" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="36"/>
-    </row>
-    <row r="17" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="36"/>
-    </row>
-    <row r="18" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="102"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="97"/>
-      <c r="M18" s="36"/>
-    </row>
-    <row r="19" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="96"/>
+    <row r="13" spans="1:15" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="89" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="89" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="130" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="131"/>
+      <c r="M13" s="132" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="139" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="135" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="135"/>
+      <c r="K14" s="135"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="139" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="135" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="135"/>
+      <c r="K15" s="135"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="133" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="140" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="134" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="133" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="136"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="138" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="133" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="140" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="134" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="133" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="136"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="135"/>
+      <c r="K18" s="135"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="136" t="s">
+        <v>22</v>
+      </c>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="38"/>
-    </row>
-    <row r="20" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="96"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="95" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="136" t="s">
+        <v>22</v>
+      </c>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
-      <c r="L20" s="104"/>
-      <c r="M20" s="36"/>
-    </row>
-    <row r="21" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="35"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="95" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="136" t="s">
+        <v>22</v>
+      </c>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="38"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="36" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
@@ -2250,72 +2557,72 @@
       <c r="E22" s="14"/>
       <c r="F22" s="19"/>
       <c r="G22" s="88"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="35"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="135"/>
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
-      <c r="L22" s="104"/>
+      <c r="L22" s="98"/>
       <c r="M22" s="36"/>
     </row>
     <row r="23" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="81"/>
-      <c r="B23" s="81"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="84"/>
       <c r="D23" s="85"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="26"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="38"/>
     </row>
     <row r="24" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="84"/>
       <c r="D24" s="85"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="24"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="36"/>
     </row>
     <row r="25" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="22"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="87"/>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
       <c r="K25" s="23"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="24"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="26"/>
     </row>
     <row r="26" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="25"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="86"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="26"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
@@ -2338,14 +2645,14 @@
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="22"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="24"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="26"/>
     </row>
     <row r="29" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
@@ -2353,14 +2660,14 @@
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="25"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="26"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
@@ -2383,14 +2690,14 @@
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="22"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="24"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
@@ -2413,14 +2720,14 @@
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
       <c r="E33" s="19"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="25"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
       <c r="K33" s="23"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="26"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
@@ -2443,14 +2750,14 @@
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
       <c r="E35" s="19"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="22"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="25"/>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
       <c r="K35" s="23"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="24"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="26"/>
     </row>
     <row r="36" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
@@ -2458,14 +2765,14 @@
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="25"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="23"/>
       <c r="J36" s="23"/>
       <c r="K36" s="23"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="26"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="24"/>
     </row>
     <row r="37" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
@@ -2488,14 +2795,14 @@
       <c r="C38" s="20"/>
       <c r="D38" s="21"/>
       <c r="E38" s="19"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="22"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="25"/>
       <c r="I38" s="23"/>
       <c r="J38" s="23"/>
       <c r="K38" s="23"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="24"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="26"/>
     </row>
     <row r="39" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
@@ -2503,14 +2810,14 @@
       <c r="C39" s="20"/>
       <c r="D39" s="21"/>
       <c r="E39" s="19"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="25"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="23"/>
       <c r="J39" s="23"/>
       <c r="K39" s="23"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="26"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="24"/>
     </row>
     <row r="40" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="16"/>
@@ -2533,14 +2840,14 @@
       <c r="C41" s="20"/>
       <c r="D41" s="21"/>
       <c r="E41" s="19"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="22"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="23"/>
       <c r="J41" s="23"/>
       <c r="K41" s="23"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="24"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="26"/>
     </row>
     <row r="42" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="16"/>
@@ -2548,19 +2855,19 @@
       <c r="C42" s="20"/>
       <c r="D42" s="21"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="25"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="23"/>
       <c r="J42" s="23"/>
       <c r="K42" s="23"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="26"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="24"/>
     </row>
     <row r="43" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="27"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="21"/>
       <c r="E43" s="19"/>
       <c r="F43" s="17"/>
@@ -2590,7 +2897,7 @@
     <row r="45" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="20"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="21"/>
       <c r="E45" s="19"/>
       <c r="F45" s="17"/>
@@ -2608,14 +2915,14 @@
       <c r="C46" s="20"/>
       <c r="D46" s="21"/>
       <c r="E46" s="19"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="22"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="25"/>
       <c r="I46" s="23"/>
       <c r="J46" s="23"/>
       <c r="K46" s="23"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="24"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="26"/>
     </row>
     <row r="47" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
@@ -2623,14 +2930,14 @@
       <c r="C47" s="20"/>
       <c r="D47" s="21"/>
       <c r="E47" s="19"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="25"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="22"/>
       <c r="I47" s="23"/>
       <c r="J47" s="23"/>
       <c r="K47" s="23"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="26"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="24"/>
     </row>
     <row r="48" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
@@ -2653,14 +2960,14 @@
       <c r="C49" s="20"/>
       <c r="D49" s="21"/>
       <c r="E49" s="19"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="22"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="25"/>
       <c r="I49" s="23"/>
       <c r="J49" s="23"/>
       <c r="K49" s="23"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="24"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="26"/>
     </row>
     <row r="50" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
@@ -2668,14 +2975,14 @@
       <c r="C50" s="20"/>
       <c r="D50" s="21"/>
       <c r="E50" s="19"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="25"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="22"/>
       <c r="I50" s="23"/>
       <c r="J50" s="23"/>
       <c r="K50" s="23"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="26"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="24"/>
     </row>
     <row r="51" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
@@ -2698,14 +3005,14 @@
       <c r="C52" s="20"/>
       <c r="D52" s="21"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="22"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="25"/>
       <c r="I52" s="23"/>
       <c r="J52" s="23"/>
       <c r="K52" s="23"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="24"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="26"/>
     </row>
     <row r="53" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="16"/>
@@ -2713,14 +3020,14 @@
       <c r="C53" s="20"/>
       <c r="D53" s="21"/>
       <c r="E53" s="19"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="25"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="22"/>
       <c r="I53" s="23"/>
       <c r="J53" s="23"/>
       <c r="K53" s="23"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="26"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="24"/>
     </row>
     <row r="54" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
@@ -2743,14 +3050,14 @@
       <c r="C55" s="20"/>
       <c r="D55" s="21"/>
       <c r="E55" s="19"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="22"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="25"/>
       <c r="I55" s="23"/>
       <c r="J55" s="23"/>
       <c r="K55" s="23"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="24"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="26"/>
     </row>
     <row r="56" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
@@ -2758,14 +3065,14 @@
       <c r="C56" s="20"/>
       <c r="D56" s="21"/>
       <c r="E56" s="19"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="25"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="22"/>
       <c r="I56" s="23"/>
       <c r="J56" s="23"/>
       <c r="K56" s="23"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="26"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="24"/>
     </row>
     <row r="57" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
@@ -2788,14 +3095,14 @@
       <c r="C58" s="20"/>
       <c r="D58" s="21"/>
       <c r="E58" s="19"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="22"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="25"/>
       <c r="I58" s="23"/>
       <c r="J58" s="23"/>
       <c r="K58" s="23"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="24"/>
+      <c r="L58" s="25"/>
+      <c r="M58" s="26"/>
     </row>
     <row r="59" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
@@ -2803,14 +3110,14 @@
       <c r="C59" s="20"/>
       <c r="D59" s="21"/>
       <c r="E59" s="19"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="25"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="22"/>
       <c r="I59" s="23"/>
       <c r="J59" s="23"/>
       <c r="K59" s="23"/>
-      <c r="L59" s="25"/>
-      <c r="M59" s="26"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="24"/>
     </row>
     <row r="60" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
@@ -2833,14 +3140,14 @@
       <c r="C61" s="20"/>
       <c r="D61" s="21"/>
       <c r="E61" s="19"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="22"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="25"/>
       <c r="I61" s="23"/>
       <c r="J61" s="23"/>
       <c r="K61" s="23"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="24"/>
+      <c r="L61" s="25"/>
+      <c r="M61" s="26"/>
     </row>
     <row r="62" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
@@ -2848,14 +3155,14 @@
       <c r="C62" s="20"/>
       <c r="D62" s="21"/>
       <c r="E62" s="19"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="25"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="22"/>
       <c r="I62" s="23"/>
       <c r="J62" s="23"/>
       <c r="K62" s="23"/>
-      <c r="L62" s="25"/>
-      <c r="M62" s="26"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="24"/>
     </row>
     <row r="63" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
@@ -2878,14 +3185,14 @@
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
       <c r="E64" s="19"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="22"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="25"/>
       <c r="I64" s="23"/>
       <c r="J64" s="23"/>
       <c r="K64" s="23"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="24"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="26"/>
     </row>
     <row r="65" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
@@ -3170,7 +3477,7 @@
       <c r="J83" s="23"/>
       <c r="K83" s="23"/>
       <c r="L83" s="22"/>
-      <c r="M83" s="26"/>
+      <c r="M83" s="24"/>
     </row>
     <row r="84" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
@@ -3185,7 +3492,7 @@
       <c r="J84" s="23"/>
       <c r="K84" s="23"/>
       <c r="L84" s="22"/>
-      <c r="M84" s="26"/>
+      <c r="M84" s="24"/>
     </row>
     <row r="85" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
@@ -3215,7 +3522,7 @@
       <c r="J86" s="23"/>
       <c r="K86" s="23"/>
       <c r="L86" s="22"/>
-      <c r="M86" s="24"/>
+      <c r="M86" s="26"/>
     </row>
     <row r="87" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
@@ -3230,7 +3537,7 @@
       <c r="J87" s="23"/>
       <c r="K87" s="23"/>
       <c r="L87" s="22"/>
-      <c r="M87" s="24"/>
+      <c r="M87" s="26"/>
     </row>
     <row r="88" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
@@ -3712,10 +4019,10 @@
       <c r="L119" s="22"/>
       <c r="M119" s="24"/>
     </row>
-    <row r="120" spans="1:13" s="15" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="16"/>
       <c r="B120" s="16"/>
-      <c r="C120" s="27"/>
+      <c r="C120" s="20"/>
       <c r="D120" s="21"/>
       <c r="E120" s="19"/>
       <c r="F120" s="17"/>
@@ -3742,10 +4049,10 @@
       <c r="L121" s="22"/>
       <c r="M121" s="24"/>
     </row>
-    <row r="122" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" s="15" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="16"/>
       <c r="B122" s="16"/>
-      <c r="C122" s="20"/>
+      <c r="C122" s="27"/>
       <c r="D122" s="21"/>
       <c r="E122" s="19"/>
       <c r="F122" s="17"/>
@@ -3772,7 +4079,7 @@
       <c r="L123" s="22"/>
       <c r="M123" s="24"/>
     </row>
-    <row r="124" spans="1:13" s="15" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="16"/>
       <c r="B124" s="16"/>
       <c r="C124" s="20"/>
@@ -3802,10 +4109,10 @@
       <c r="L125" s="22"/>
       <c r="M125" s="24"/>
     </row>
-    <row r="126" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" s="15" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="16"/>
       <c r="B126" s="16"/>
-      <c r="C126" s="27"/>
+      <c r="C126" s="20"/>
       <c r="D126" s="21"/>
       <c r="E126" s="19"/>
       <c r="F126" s="17"/>
@@ -3835,7 +4142,7 @@
     <row r="128" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="16"/>
       <c r="B128" s="16"/>
-      <c r="C128" s="20"/>
+      <c r="C128" s="27"/>
       <c r="D128" s="21"/>
       <c r="E128" s="19"/>
       <c r="F128" s="17"/>
@@ -3973,9 +4280,9 @@
       <c r="C137" s="20"/>
       <c r="D137" s="21"/>
       <c r="E137" s="19"/>
-      <c r="F137" s="28"/>
-      <c r="G137" s="16"/>
-      <c r="H137" s="29"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="18"/>
+      <c r="H137" s="22"/>
       <c r="I137" s="23"/>
       <c r="J137" s="23"/>
       <c r="K137" s="23"/>
@@ -3988,7 +4295,7 @@
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
       <c r="E138" s="19"/>
-      <c r="F138" s="28"/>
+      <c r="F138" s="17"/>
       <c r="G138" s="18"/>
       <c r="H138" s="22"/>
       <c r="I138" s="23"/>
@@ -4005,7 +4312,7 @@
       <c r="E139" s="19"/>
       <c r="F139" s="28"/>
       <c r="G139" s="16"/>
-      <c r="H139" s="22"/>
+      <c r="H139" s="29"/>
       <c r="I139" s="23"/>
       <c r="J139" s="23"/>
       <c r="K139" s="23"/>
@@ -4019,7 +4326,7 @@
       <c r="D140" s="21"/>
       <c r="E140" s="19"/>
       <c r="F140" s="28"/>
-      <c r="G140" s="16"/>
+      <c r="G140" s="18"/>
       <c r="H140" s="22"/>
       <c r="I140" s="23"/>
       <c r="J140" s="23"/>
@@ -4050,7 +4357,7 @@
       <c r="E142" s="19"/>
       <c r="F142" s="28"/>
       <c r="G142" s="16"/>
-      <c r="H142" s="29"/>
+      <c r="H142" s="22"/>
       <c r="I142" s="23"/>
       <c r="J142" s="23"/>
       <c r="K142" s="23"/>
@@ -4070,7 +4377,7 @@
       <c r="J143" s="23"/>
       <c r="K143" s="23"/>
       <c r="L143" s="22"/>
-      <c r="M143" s="26"/>
+      <c r="M143" s="24"/>
     </row>
     <row r="144" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="16"/>
@@ -4080,7 +4387,7 @@
       <c r="E144" s="19"/>
       <c r="F144" s="28"/>
       <c r="G144" s="16"/>
-      <c r="H144" s="22"/>
+      <c r="H144" s="29"/>
       <c r="I144" s="23"/>
       <c r="J144" s="23"/>
       <c r="K144" s="23"/>
@@ -4100,7 +4407,7 @@
       <c r="J145" s="23"/>
       <c r="K145" s="23"/>
       <c r="L145" s="22"/>
-      <c r="M145" s="24"/>
+      <c r="M145" s="26"/>
     </row>
     <row r="146" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="16"/>
@@ -4123,8 +4430,8 @@
       <c r="C147" s="20"/>
       <c r="D147" s="21"/>
       <c r="E147" s="19"/>
-      <c r="F147" s="17"/>
-      <c r="G147" s="18"/>
+      <c r="F147" s="28"/>
+      <c r="G147" s="16"/>
       <c r="H147" s="22"/>
       <c r="I147" s="23"/>
       <c r="J147" s="23"/>
@@ -4138,8 +4445,8 @@
       <c r="C148" s="20"/>
       <c r="D148" s="21"/>
       <c r="E148" s="19"/>
-      <c r="F148" s="17"/>
-      <c r="G148" s="18"/>
+      <c r="F148" s="28"/>
+      <c r="G148" s="16"/>
       <c r="H148" s="22"/>
       <c r="I148" s="23"/>
       <c r="J148" s="23"/>
@@ -4288,7 +4595,7 @@
       <c r="C158" s="20"/>
       <c r="D158" s="21"/>
       <c r="E158" s="19"/>
-      <c r="F158" s="30"/>
+      <c r="F158" s="17"/>
       <c r="G158" s="18"/>
       <c r="H158" s="22"/>
       <c r="I158" s="23"/>
@@ -4318,7 +4625,7 @@
       <c r="C160" s="20"/>
       <c r="D160" s="21"/>
       <c r="E160" s="19"/>
-      <c r="F160" s="17"/>
+      <c r="F160" s="30"/>
       <c r="G160" s="18"/>
       <c r="H160" s="22"/>
       <c r="I160" s="23"/>
@@ -4462,35 +4769,35 @@
       <c r="L169" s="22"/>
       <c r="M169" s="24"/>
     </row>
-    <row r="170" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A170" s="31"/>
-      <c r="B170" s="31"/>
+    <row r="170" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A170" s="16"/>
+      <c r="B170" s="16"/>
       <c r="C170" s="20"/>
       <c r="D170" s="21"/>
       <c r="E170" s="19"/>
-      <c r="F170" s="32"/>
-      <c r="G170" s="33"/>
-      <c r="H170" s="34"/>
-      <c r="I170" s="35"/>
-      <c r="J170" s="35"/>
-      <c r="K170" s="35"/>
-      <c r="L170" s="34"/>
-      <c r="M170" s="36"/>
-    </row>
-    <row r="171" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A171" s="31"/>
-      <c r="B171" s="31"/>
+      <c r="F170" s="17"/>
+      <c r="G170" s="18"/>
+      <c r="H170" s="22"/>
+      <c r="I170" s="23"/>
+      <c r="J170" s="23"/>
+      <c r="K170" s="23"/>
+      <c r="L170" s="22"/>
+      <c r="M170" s="24"/>
+    </row>
+    <row r="171" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A171" s="16"/>
+      <c r="B171" s="16"/>
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
       <c r="E171" s="19"/>
-      <c r="F171" s="32"/>
-      <c r="G171" s="33"/>
-      <c r="H171" s="34"/>
-      <c r="I171" s="35"/>
-      <c r="J171" s="35"/>
-      <c r="K171" s="35"/>
-      <c r="L171" s="34"/>
-      <c r="M171" s="36"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="18"/>
+      <c r="H171" s="22"/>
+      <c r="I171" s="23"/>
+      <c r="J171" s="23"/>
+      <c r="K171" s="23"/>
+      <c r="L171" s="22"/>
+      <c r="M171" s="24"/>
     </row>
     <row r="172" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A172" s="31"/>
@@ -4529,7 +4836,7 @@
       <c r="D174" s="21"/>
       <c r="E174" s="19"/>
       <c r="F174" s="32"/>
-      <c r="G174" s="31"/>
+      <c r="G174" s="33"/>
       <c r="H174" s="34"/>
       <c r="I174" s="35"/>
       <c r="J174" s="35"/>
@@ -4559,7 +4866,7 @@
       <c r="D176" s="21"/>
       <c r="E176" s="19"/>
       <c r="F176" s="32"/>
-      <c r="G176" s="33"/>
+      <c r="G176" s="31"/>
       <c r="H176" s="34"/>
       <c r="I176" s="35"/>
       <c r="J176" s="35"/>
@@ -4720,7 +5027,7 @@
     <row r="187" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A187" s="31"/>
       <c r="B187" s="31"/>
-      <c r="C187" s="32"/>
+      <c r="C187" s="20"/>
       <c r="D187" s="21"/>
       <c r="E187" s="19"/>
       <c r="F187" s="32"/>
@@ -4735,7 +5042,7 @@
     <row r="188" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A188" s="31"/>
       <c r="B188" s="31"/>
-      <c r="C188" s="32"/>
+      <c r="C188" s="20"/>
       <c r="D188" s="21"/>
       <c r="E188" s="19"/>
       <c r="F188" s="32"/>
@@ -4751,7 +5058,7 @@
       <c r="A189" s="31"/>
       <c r="B189" s="31"/>
       <c r="C189" s="32"/>
-      <c r="D189" s="33"/>
+      <c r="D189" s="21"/>
       <c r="E189" s="19"/>
       <c r="F189" s="32"/>
       <c r="G189" s="33"/>
@@ -4766,7 +5073,7 @@
       <c r="A190" s="31"/>
       <c r="B190" s="31"/>
       <c r="C190" s="32"/>
-      <c r="D190" s="33"/>
+      <c r="D190" s="21"/>
       <c r="E190" s="19"/>
       <c r="F190" s="32"/>
       <c r="G190" s="33"/>
@@ -4783,7 +5090,7 @@
       <c r="C191" s="32"/>
       <c r="D191" s="33"/>
       <c r="E191" s="19"/>
-      <c r="F191" s="37"/>
+      <c r="F191" s="32"/>
       <c r="G191" s="33"/>
       <c r="H191" s="34"/>
       <c r="I191" s="35"/>
@@ -4813,7 +5120,7 @@
       <c r="C193" s="32"/>
       <c r="D193" s="33"/>
       <c r="E193" s="19"/>
-      <c r="F193" s="32"/>
+      <c r="F193" s="37"/>
       <c r="G193" s="33"/>
       <c r="H193" s="34"/>
       <c r="I193" s="35"/>
@@ -4994,7 +5301,7 @@
       <c r="D205" s="33"/>
       <c r="E205" s="19"/>
       <c r="F205" s="32"/>
-      <c r="G205" s="31"/>
+      <c r="G205" s="33"/>
       <c r="H205" s="34"/>
       <c r="I205" s="35"/>
       <c r="J205" s="35"/>
@@ -5024,7 +5331,7 @@
       <c r="D207" s="33"/>
       <c r="E207" s="19"/>
       <c r="F207" s="32"/>
-      <c r="G207" s="33"/>
+      <c r="G207" s="31"/>
       <c r="H207" s="34"/>
       <c r="I207" s="35"/>
       <c r="J207" s="35"/>
@@ -5084,7 +5391,7 @@
       <c r="D211" s="33"/>
       <c r="E211" s="19"/>
       <c r="F211" s="32"/>
-      <c r="G211" s="31"/>
+      <c r="G211" s="33"/>
       <c r="H211" s="34"/>
       <c r="I211" s="35"/>
       <c r="J211" s="35"/>
@@ -5114,7 +5421,7 @@
       <c r="D213" s="33"/>
       <c r="E213" s="19"/>
       <c r="F213" s="32"/>
-      <c r="G213" s="33"/>
+      <c r="G213" s="31"/>
       <c r="H213" s="34"/>
       <c r="I213" s="35"/>
       <c r="J213" s="35"/>
@@ -5135,7 +5442,7 @@
       <c r="J214" s="35"/>
       <c r="K214" s="35"/>
       <c r="L214" s="34"/>
-      <c r="M214" s="38"/>
+      <c r="M214" s="36"/>
     </row>
     <row r="215" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A215" s="31"/>
@@ -5165,7 +5472,7 @@
       <c r="J216" s="35"/>
       <c r="K216" s="35"/>
       <c r="L216" s="34"/>
-      <c r="M216" s="36"/>
+      <c r="M216" s="38"/>
     </row>
     <row r="217" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A217" s="31"/>
@@ -5204,7 +5511,7 @@
       <c r="D219" s="33"/>
       <c r="E219" s="19"/>
       <c r="F219" s="32"/>
-      <c r="G219" s="31"/>
+      <c r="G219" s="33"/>
       <c r="H219" s="34"/>
       <c r="I219" s="35"/>
       <c r="J219" s="35"/>
@@ -5215,11 +5522,11 @@
     <row r="220" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A220" s="31"/>
       <c r="B220" s="31"/>
-      <c r="C220" s="39"/>
+      <c r="C220" s="32"/>
       <c r="D220" s="33"/>
       <c r="E220" s="19"/>
       <c r="F220" s="32"/>
-      <c r="G220" s="31"/>
+      <c r="G220" s="33"/>
       <c r="H220" s="34"/>
       <c r="I220" s="35"/>
       <c r="J220" s="35"/>
@@ -5230,11 +5537,11 @@
     <row r="221" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A221" s="31"/>
       <c r="B221" s="31"/>
-      <c r="C221" s="39"/>
+      <c r="C221" s="32"/>
       <c r="D221" s="33"/>
       <c r="E221" s="19"/>
       <c r="F221" s="32"/>
-      <c r="G221" s="33"/>
+      <c r="G221" s="31"/>
       <c r="H221" s="34"/>
       <c r="I221" s="35"/>
       <c r="J221" s="35"/>
@@ -5242,35 +5549,35 @@
       <c r="L221" s="34"/>
       <c r="M221" s="36"/>
     </row>
-    <row r="222" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A222" s="40"/>
-      <c r="B222" s="40"/>
+    <row r="222" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A222" s="31"/>
+      <c r="B222" s="31"/>
       <c r="C222" s="39"/>
-      <c r="D222" s="41"/>
+      <c r="D222" s="33"/>
       <c r="E222" s="19"/>
-      <c r="F222" s="39"/>
-      <c r="G222" s="41"/>
-      <c r="H222" s="42"/>
-      <c r="I222" s="43"/>
-      <c r="J222" s="43"/>
-      <c r="K222" s="43"/>
-      <c r="L222" s="42"/>
-      <c r="M222" s="44"/>
-    </row>
-    <row r="223" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A223" s="40"/>
-      <c r="B223" s="40"/>
+      <c r="F222" s="32"/>
+      <c r="G222" s="31"/>
+      <c r="H222" s="34"/>
+      <c r="I222" s="35"/>
+      <c r="J222" s="35"/>
+      <c r="K222" s="35"/>
+      <c r="L222" s="34"/>
+      <c r="M222" s="36"/>
+    </row>
+    <row r="223" spans="1:13" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A223" s="31"/>
+      <c r="B223" s="31"/>
       <c r="C223" s="39"/>
-      <c r="D223" s="41"/>
+      <c r="D223" s="33"/>
       <c r="E223" s="19"/>
-      <c r="F223" s="39"/>
-      <c r="G223" s="41"/>
-      <c r="H223" s="42"/>
-      <c r="I223" s="43"/>
-      <c r="J223" s="43"/>
-      <c r="K223" s="43"/>
-      <c r="L223" s="42"/>
-      <c r="M223" s="44"/>
+      <c r="F223" s="32"/>
+      <c r="G223" s="33"/>
+      <c r="H223" s="34"/>
+      <c r="I223" s="35"/>
+      <c r="J223" s="35"/>
+      <c r="K223" s="35"/>
+      <c r="L223" s="34"/>
+      <c r="M223" s="36"/>
     </row>
     <row r="224" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A224" s="40"/>
@@ -5398,7 +5705,7 @@
       <c r="C232" s="39"/>
       <c r="D232" s="41"/>
       <c r="E232" s="19"/>
-      <c r="F232" s="45"/>
+      <c r="F232" s="39"/>
       <c r="G232" s="41"/>
       <c r="H232" s="42"/>
       <c r="I232" s="43"/>
@@ -5420,7 +5727,7 @@
       <c r="J233" s="43"/>
       <c r="K233" s="43"/>
       <c r="L233" s="42"/>
-      <c r="M233" s="46"/>
+      <c r="M233" s="44"/>
     </row>
     <row r="234" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A234" s="40"/>
@@ -5428,7 +5735,7 @@
       <c r="C234" s="39"/>
       <c r="D234" s="41"/>
       <c r="E234" s="19"/>
-      <c r="F234" s="39"/>
+      <c r="F234" s="45"/>
       <c r="G234" s="41"/>
       <c r="H234" s="42"/>
       <c r="I234" s="43"/>
@@ -5450,7 +5757,7 @@
       <c r="J235" s="43"/>
       <c r="K235" s="43"/>
       <c r="L235" s="42"/>
-      <c r="M235" s="44"/>
+      <c r="M235" s="46"/>
     </row>
     <row r="236" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A236" s="40"/>
@@ -5465,7 +5772,7 @@
       <c r="J236" s="43"/>
       <c r="K236" s="43"/>
       <c r="L236" s="42"/>
-      <c r="M236" s="46"/>
+      <c r="M236" s="44"/>
     </row>
     <row r="237" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A237" s="40"/>
@@ -5495,7 +5802,7 @@
       <c r="J238" s="43"/>
       <c r="K238" s="43"/>
       <c r="L238" s="42"/>
-      <c r="M238" s="44"/>
+      <c r="M238" s="46"/>
     </row>
     <row r="239" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A239" s="40"/>
@@ -5525,7 +5832,7 @@
       <c r="J240" s="43"/>
       <c r="K240" s="43"/>
       <c r="L240" s="42"/>
-      <c r="M240" s="46"/>
+      <c r="M240" s="44"/>
     </row>
     <row r="241" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A241" s="40"/>
@@ -5555,7 +5862,7 @@
       <c r="J242" s="43"/>
       <c r="K242" s="43"/>
       <c r="L242" s="42"/>
-      <c r="M242" s="44"/>
+      <c r="M242" s="46"/>
     </row>
     <row r="243" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A243" s="40"/>
@@ -5570,7 +5877,7 @@
       <c r="J243" s="43"/>
       <c r="K243" s="43"/>
       <c r="L243" s="42"/>
-      <c r="M243" s="46"/>
+      <c r="M243" s="44"/>
     </row>
     <row r="244" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A244" s="40"/>
@@ -5600,7 +5907,7 @@
       <c r="J245" s="43"/>
       <c r="K245" s="43"/>
       <c r="L245" s="42"/>
-      <c r="M245" s="44"/>
+      <c r="M245" s="46"/>
     </row>
     <row r="246" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A246" s="40"/>
@@ -5983,9 +6290,9 @@
       <c r="C271" s="39"/>
       <c r="D271" s="41"/>
       <c r="E271" s="19"/>
-      <c r="F271" s="47"/>
+      <c r="F271" s="39"/>
       <c r="G271" s="41"/>
-      <c r="H271" s="48"/>
+      <c r="H271" s="42"/>
       <c r="I271" s="43"/>
       <c r="J271" s="43"/>
       <c r="K271" s="43"/>
@@ -5998,9 +6305,9 @@
       <c r="C272" s="39"/>
       <c r="D272" s="41"/>
       <c r="E272" s="19"/>
-      <c r="F272" s="47"/>
-      <c r="G272" s="40"/>
-      <c r="H272" s="48"/>
+      <c r="F272" s="39"/>
+      <c r="G272" s="41"/>
+      <c r="H272" s="42"/>
       <c r="I272" s="43"/>
       <c r="J272" s="43"/>
       <c r="K272" s="43"/>
@@ -6043,9 +6350,9 @@
       <c r="C275" s="39"/>
       <c r="D275" s="41"/>
       <c r="E275" s="19"/>
-      <c r="F275" s="39"/>
-      <c r="G275" s="42"/>
-      <c r="H275" s="42"/>
+      <c r="F275" s="47"/>
+      <c r="G275" s="41"/>
+      <c r="H275" s="48"/>
       <c r="I275" s="43"/>
       <c r="J275" s="43"/>
       <c r="K275" s="43"/>
@@ -6058,9 +6365,9 @@
       <c r="C276" s="39"/>
       <c r="D276" s="41"/>
       <c r="E276" s="19"/>
-      <c r="F276" s="39"/>
-      <c r="G276" s="41"/>
-      <c r="H276" s="42"/>
+      <c r="F276" s="47"/>
+      <c r="G276" s="40"/>
+      <c r="H276" s="48"/>
       <c r="I276" s="43"/>
       <c r="J276" s="43"/>
       <c r="K276" s="43"/>
@@ -6074,7 +6381,7 @@
       <c r="D277" s="41"/>
       <c r="E277" s="19"/>
       <c r="F277" s="39"/>
-      <c r="G277" s="41"/>
+      <c r="G277" s="42"/>
       <c r="H277" s="42"/>
       <c r="I277" s="43"/>
       <c r="J277" s="43"/>
@@ -6095,7 +6402,7 @@
       <c r="J278" s="43"/>
       <c r="K278" s="43"/>
       <c r="L278" s="42"/>
-      <c r="M278" s="46"/>
+      <c r="M278" s="44"/>
     </row>
     <row r="279" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A279" s="40"/>
@@ -6155,7 +6462,7 @@
       <c r="J282" s="43"/>
       <c r="K282" s="43"/>
       <c r="L282" s="42"/>
-      <c r="M282" s="44"/>
+      <c r="M282" s="46"/>
     </row>
     <row r="283" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A283" s="40"/>
@@ -6215,7 +6522,7 @@
       <c r="J286" s="43"/>
       <c r="K286" s="43"/>
       <c r="L286" s="42"/>
-      <c r="M286" s="46"/>
+      <c r="M286" s="44"/>
     </row>
     <row r="287" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A287" s="40"/>
@@ -6245,7 +6552,7 @@
       <c r="J288" s="43"/>
       <c r="K288" s="43"/>
       <c r="L288" s="42"/>
-      <c r="M288" s="44"/>
+      <c r="M288" s="46"/>
     </row>
     <row r="289" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A289" s="40"/>
@@ -7783,7 +8090,7 @@
       <c r="C391" s="39"/>
       <c r="D391" s="41"/>
       <c r="E391" s="19"/>
-      <c r="F391" s="1"/>
+      <c r="F391" s="39"/>
       <c r="G391" s="41"/>
       <c r="H391" s="42"/>
       <c r="I391" s="43"/>
@@ -7798,7 +8105,7 @@
       <c r="C392" s="39"/>
       <c r="D392" s="41"/>
       <c r="E392" s="19"/>
-      <c r="F392" s="47"/>
+      <c r="F392" s="39"/>
       <c r="G392" s="41"/>
       <c r="H392" s="42"/>
       <c r="I392" s="43"/>
@@ -7813,7 +8120,7 @@
       <c r="C393" s="39"/>
       <c r="D393" s="41"/>
       <c r="E393" s="19"/>
-      <c r="F393" s="47"/>
+      <c r="F393" s="1"/>
       <c r="G393" s="41"/>
       <c r="H393" s="42"/>
       <c r="I393" s="43"/>
@@ -7837,35 +8144,35 @@
       <c r="L394" s="42"/>
       <c r="M394" s="44"/>
     </row>
-    <row r="395" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A395" s="49"/>
-      <c r="B395" s="49"/>
-      <c r="C395" s="50"/>
-      <c r="D395" s="51"/>
+    <row r="395" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A395" s="40"/>
+      <c r="B395" s="40"/>
+      <c r="C395" s="39"/>
+      <c r="D395" s="41"/>
       <c r="E395" s="19"/>
-      <c r="F395" s="52"/>
-      <c r="G395" s="52"/>
-      <c r="H395" s="49"/>
-      <c r="I395" s="53"/>
-      <c r="J395" s="53"/>
-      <c r="K395" s="53"/>
-      <c r="L395" s="49"/>
-      <c r="M395" s="54"/>
-    </row>
-    <row r="396" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A396" s="49"/>
-      <c r="B396" s="49"/>
-      <c r="C396" s="50"/>
-      <c r="D396" s="51"/>
+      <c r="F395" s="47"/>
+      <c r="G395" s="41"/>
+      <c r="H395" s="42"/>
+      <c r="I395" s="43"/>
+      <c r="J395" s="43"/>
+      <c r="K395" s="43"/>
+      <c r="L395" s="42"/>
+      <c r="M395" s="44"/>
+    </row>
+    <row r="396" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A396" s="40"/>
+      <c r="B396" s="40"/>
+      <c r="C396" s="39"/>
+      <c r="D396" s="41"/>
       <c r="E396" s="19"/>
-      <c r="F396" s="52"/>
-      <c r="G396" s="52"/>
-      <c r="H396" s="49"/>
-      <c r="I396" s="53"/>
-      <c r="J396" s="53"/>
-      <c r="K396" s="53"/>
-      <c r="L396" s="49"/>
-      <c r="M396" s="54"/>
+      <c r="F396" s="47"/>
+      <c r="G396" s="41"/>
+      <c r="H396" s="42"/>
+      <c r="I396" s="43"/>
+      <c r="J396" s="43"/>
+      <c r="K396" s="43"/>
+      <c r="L396" s="42"/>
+      <c r="M396" s="44"/>
     </row>
     <row r="397" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A397" s="49"/>
@@ -7882,65 +8189,65 @@
       <c r="L397" s="49"/>
       <c r="M397" s="54"/>
     </row>
-    <row r="398" spans="1:13" s="61" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A398" s="56"/>
-      <c r="B398" s="56"/>
-      <c r="C398" s="57"/>
-      <c r="D398" s="58"/>
+    <row r="398" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A398" s="49"/>
+      <c r="B398" s="49"/>
+      <c r="C398" s="50"/>
+      <c r="D398" s="51"/>
       <c r="E398" s="19"/>
       <c r="F398" s="52"/>
       <c r="G398" s="52"/>
       <c r="H398" s="49"/>
-      <c r="I398" s="59"/>
-      <c r="J398" s="59"/>
-      <c r="K398" s="59"/>
-      <c r="L398" s="56"/>
-      <c r="M398" s="60"/>
-    </row>
-    <row r="399" spans="1:13" s="61" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A399" s="56"/>
-      <c r="B399" s="56"/>
-      <c r="C399" s="57"/>
-      <c r="D399" s="58"/>
+      <c r="I398" s="53"/>
+      <c r="J398" s="53"/>
+      <c r="K398" s="53"/>
+      <c r="L398" s="49"/>
+      <c r="M398" s="54"/>
+    </row>
+    <row r="399" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A399" s="49"/>
+      <c r="B399" s="49"/>
+      <c r="C399" s="50"/>
+      <c r="D399" s="51"/>
       <c r="E399" s="19"/>
       <c r="F399" s="52"/>
       <c r="G399" s="52"/>
       <c r="H399" s="49"/>
-      <c r="I399" s="59"/>
-      <c r="J399" s="59"/>
-      <c r="K399" s="59"/>
-      <c r="L399" s="56"/>
-      <c r="M399" s="60"/>
-    </row>
-    <row r="400" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A400" s="49"/>
-      <c r="B400" s="49"/>
-      <c r="C400" s="50"/>
-      <c r="D400" s="51"/>
+      <c r="I399" s="53"/>
+      <c r="J399" s="53"/>
+      <c r="K399" s="53"/>
+      <c r="L399" s="49"/>
+      <c r="M399" s="54"/>
+    </row>
+    <row r="400" spans="1:13" s="61" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A400" s="56"/>
+      <c r="B400" s="56"/>
+      <c r="C400" s="57"/>
+      <c r="D400" s="58"/>
       <c r="E400" s="19"/>
       <c r="F400" s="52"/>
       <c r="G400" s="52"/>
       <c r="H400" s="49"/>
-      <c r="I400" s="53"/>
-      <c r="J400" s="53"/>
-      <c r="K400" s="53"/>
-      <c r="L400" s="49"/>
-      <c r="M400" s="54"/>
-    </row>
-    <row r="401" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A401" s="49"/>
-      <c r="B401" s="49"/>
-      <c r="C401" s="50"/>
-      <c r="D401" s="51"/>
+      <c r="I400" s="59"/>
+      <c r="J400" s="59"/>
+      <c r="K400" s="59"/>
+      <c r="L400" s="56"/>
+      <c r="M400" s="60"/>
+    </row>
+    <row r="401" spans="1:13" s="61" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A401" s="56"/>
+      <c r="B401" s="56"/>
+      <c r="C401" s="57"/>
+      <c r="D401" s="58"/>
       <c r="E401" s="19"/>
       <c r="F401" s="52"/>
       <c r="G401" s="52"/>
       <c r="H401" s="49"/>
-      <c r="I401" s="53"/>
-      <c r="J401" s="53"/>
-      <c r="K401" s="53"/>
-      <c r="L401" s="49"/>
-      <c r="M401" s="54"/>
+      <c r="I401" s="59"/>
+      <c r="J401" s="59"/>
+      <c r="K401" s="59"/>
+      <c r="L401" s="56"/>
+      <c r="M401" s="60"/>
     </row>
     <row r="402" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A402" s="49"/>
@@ -8182,35 +8489,35 @@
       <c r="L417" s="49"/>
       <c r="M417" s="54"/>
     </row>
-    <row r="418" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A418" s="40"/>
-      <c r="B418" s="40"/>
+    <row r="418" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A418" s="49"/>
+      <c r="B418" s="49"/>
       <c r="C418" s="50"/>
       <c r="D418" s="51"/>
       <c r="E418" s="19"/>
-      <c r="F418" s="39"/>
-      <c r="G418" s="41"/>
-      <c r="H418" s="42"/>
-      <c r="I418" s="43"/>
-      <c r="J418" s="43"/>
-      <c r="K418" s="43"/>
-      <c r="L418" s="42"/>
-      <c r="M418" s="44"/>
-    </row>
-    <row r="419" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A419" s="40"/>
-      <c r="B419" s="40"/>
+      <c r="F418" s="52"/>
+      <c r="G418" s="52"/>
+      <c r="H418" s="49"/>
+      <c r="I418" s="53"/>
+      <c r="J418" s="53"/>
+      <c r="K418" s="53"/>
+      <c r="L418" s="49"/>
+      <c r="M418" s="54"/>
+    </row>
+    <row r="419" spans="1:13" s="55" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A419" s="49"/>
+      <c r="B419" s="49"/>
       <c r="C419" s="50"/>
       <c r="D419" s="51"/>
       <c r="E419" s="19"/>
-      <c r="F419" s="39"/>
-      <c r="G419" s="41"/>
-      <c r="H419" s="42"/>
-      <c r="I419" s="43"/>
-      <c r="J419" s="43"/>
-      <c r="K419" s="43"/>
-      <c r="L419" s="42"/>
-      <c r="M419" s="44"/>
+      <c r="F419" s="52"/>
+      <c r="G419" s="52"/>
+      <c r="H419" s="49"/>
+      <c r="I419" s="53"/>
+      <c r="J419" s="53"/>
+      <c r="K419" s="53"/>
+      <c r="L419" s="49"/>
+      <c r="M419" s="54"/>
     </row>
     <row r="420" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A420" s="40"/>
@@ -8260,8 +8567,8 @@
     <row r="423" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A423" s="40"/>
       <c r="B423" s="40"/>
-      <c r="C423" s="39"/>
-      <c r="D423" s="41"/>
+      <c r="C423" s="50"/>
+      <c r="D423" s="51"/>
       <c r="E423" s="19"/>
       <c r="F423" s="39"/>
       <c r="G423" s="41"/>
@@ -8275,8 +8582,8 @@
     <row r="424" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A424" s="40"/>
       <c r="B424" s="40"/>
-      <c r="C424" s="39"/>
-      <c r="D424" s="41"/>
+      <c r="C424" s="50"/>
+      <c r="D424" s="51"/>
       <c r="E424" s="19"/>
       <c r="F424" s="39"/>
       <c r="G424" s="41"/>
@@ -8293,7 +8600,7 @@
       <c r="C425" s="39"/>
       <c r="D425" s="41"/>
       <c r="E425" s="19"/>
-      <c r="F425" s="1"/>
+      <c r="F425" s="39"/>
       <c r="G425" s="41"/>
       <c r="H425" s="42"/>
       <c r="I425" s="43"/>
@@ -8323,7 +8630,7 @@
       <c r="C427" s="39"/>
       <c r="D427" s="41"/>
       <c r="E427" s="19"/>
-      <c r="F427" s="39"/>
+      <c r="F427" s="1"/>
       <c r="G427" s="41"/>
       <c r="H427" s="42"/>
       <c r="I427" s="43"/>
@@ -8338,7 +8645,7 @@
       <c r="C428" s="39"/>
       <c r="D428" s="41"/>
       <c r="E428" s="19"/>
-      <c r="F428" s="47"/>
+      <c r="F428" s="39"/>
       <c r="G428" s="41"/>
       <c r="H428" s="42"/>
       <c r="I428" s="43"/>
@@ -8368,7 +8675,7 @@
       <c r="C430" s="39"/>
       <c r="D430" s="41"/>
       <c r="E430" s="19"/>
-      <c r="F430" s="39"/>
+      <c r="F430" s="47"/>
       <c r="G430" s="41"/>
       <c r="H430" s="42"/>
       <c r="I430" s="43"/>
@@ -9058,7 +9365,7 @@
       <c r="C476" s="39"/>
       <c r="D476" s="41"/>
       <c r="E476" s="19"/>
-      <c r="F476" s="47"/>
+      <c r="F476" s="39"/>
       <c r="G476" s="41"/>
       <c r="H476" s="42"/>
       <c r="I476" s="43"/>
@@ -9073,7 +9380,7 @@
       <c r="C477" s="39"/>
       <c r="D477" s="41"/>
       <c r="E477" s="19"/>
-      <c r="F477" s="47"/>
+      <c r="F477" s="39"/>
       <c r="G477" s="41"/>
       <c r="H477" s="42"/>
       <c r="I477" s="43"/>
@@ -9148,7 +9455,7 @@
       <c r="C482" s="39"/>
       <c r="D482" s="41"/>
       <c r="E482" s="19"/>
-      <c r="F482" s="39"/>
+      <c r="F482" s="47"/>
       <c r="G482" s="41"/>
       <c r="H482" s="42"/>
       <c r="I482" s="43"/>
@@ -9163,7 +9470,7 @@
       <c r="C483" s="39"/>
       <c r="D483" s="41"/>
       <c r="E483" s="19"/>
-      <c r="F483" s="39"/>
+      <c r="F483" s="47"/>
       <c r="G483" s="41"/>
       <c r="H483" s="42"/>
       <c r="I483" s="43"/>
@@ -9178,7 +9485,7 @@
       <c r="C484" s="39"/>
       <c r="D484" s="41"/>
       <c r="E484" s="19"/>
-      <c r="F484" s="47"/>
+      <c r="F484" s="39"/>
       <c r="G484" s="41"/>
       <c r="H484" s="42"/>
       <c r="I484" s="43"/>
@@ -9208,7 +9515,7 @@
       <c r="C486" s="39"/>
       <c r="D486" s="41"/>
       <c r="E486" s="19"/>
-      <c r="F486" s="39"/>
+      <c r="F486" s="47"/>
       <c r="G486" s="41"/>
       <c r="H486" s="42"/>
       <c r="I486" s="43"/>
@@ -9793,7 +10100,7 @@
       <c r="C525" s="39"/>
       <c r="D525" s="41"/>
       <c r="E525" s="19"/>
-      <c r="F525" s="1"/>
+      <c r="F525" s="39"/>
       <c r="G525" s="41"/>
       <c r="H525" s="42"/>
       <c r="I525" s="43"/>
@@ -9823,7 +10130,7 @@
       <c r="C527" s="39"/>
       <c r="D527" s="41"/>
       <c r="E527" s="19"/>
-      <c r="F527" s="39"/>
+      <c r="F527" s="1"/>
       <c r="G527" s="41"/>
       <c r="H527" s="42"/>
       <c r="I527" s="43"/>
@@ -9883,7 +10190,7 @@
       <c r="C531" s="39"/>
       <c r="D531" s="41"/>
       <c r="E531" s="19"/>
-      <c r="F531" s="47"/>
+      <c r="F531" s="39"/>
       <c r="G531" s="41"/>
       <c r="H531" s="42"/>
       <c r="I531" s="43"/>
@@ -9898,7 +10205,7 @@
       <c r="C532" s="39"/>
       <c r="D532" s="41"/>
       <c r="E532" s="19"/>
-      <c r="F532" s="47"/>
+      <c r="F532" s="39"/>
       <c r="G532" s="41"/>
       <c r="H532" s="42"/>
       <c r="I532" s="43"/>
@@ -9907,34 +10214,62 @@
       <c r="L532" s="42"/>
       <c r="M532" s="44"/>
     </row>
-    <row r="533" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A533" s="62"/>
-      <c r="B533" s="62"/>
-      <c r="C533" s="63"/>
-      <c r="D533" s="64"/>
-      <c r="E533" s="65"/>
-      <c r="F533" s="66"/>
-      <c r="G533" s="64"/>
-      <c r="H533" s="64"/>
-      <c r="I533" s="67"/>
-      <c r="J533" s="67"/>
-      <c r="K533" s="67"/>
-      <c r="L533" s="64"/>
-      <c r="M533" s="68"/>
-    </row>
-    <row r="534" spans="1:13" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="D534" s="69"/>
-      <c r="E534" s="70"/>
-      <c r="F534" s="69"/>
-      <c r="H534" s="9"/>
-      <c r="I534" s="71"/>
-      <c r="J534" s="71"/>
-      <c r="K534" s="71"/>
-      <c r="L534" s="72"/>
-      <c r="M534" s="72"/>
-    </row>
-    <row r="535" spans="1:13" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="536" spans="1:13" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="533" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A533" s="40"/>
+      <c r="B533" s="40"/>
+      <c r="C533" s="39"/>
+      <c r="D533" s="41"/>
+      <c r="E533" s="19"/>
+      <c r="F533" s="47"/>
+      <c r="G533" s="41"/>
+      <c r="H533" s="42"/>
+      <c r="I533" s="43"/>
+      <c r="J533" s="43"/>
+      <c r="K533" s="43"/>
+      <c r="L533" s="42"/>
+      <c r="M533" s="44"/>
+    </row>
+    <row r="534" spans="1:13" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A534" s="40"/>
+      <c r="B534" s="40"/>
+      <c r="C534" s="39"/>
+      <c r="D534" s="41"/>
+      <c r="E534" s="19"/>
+      <c r="F534" s="47"/>
+      <c r="G534" s="41"/>
+      <c r="H534" s="42"/>
+      <c r="I534" s="43"/>
+      <c r="J534" s="43"/>
+      <c r="K534" s="43"/>
+      <c r="L534" s="42"/>
+      <c r="M534" s="44"/>
+    </row>
+    <row r="535" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A535" s="62"/>
+      <c r="B535" s="62"/>
+      <c r="C535" s="63"/>
+      <c r="D535" s="64"/>
+      <c r="E535" s="65"/>
+      <c r="F535" s="66"/>
+      <c r="G535" s="64"/>
+      <c r="H535" s="64"/>
+      <c r="I535" s="67"/>
+      <c r="J535" s="67"/>
+      <c r="K535" s="67"/>
+      <c r="L535" s="64"/>
+      <c r="M535" s="68"/>
+    </row>
+    <row r="536" spans="1:13" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="D536" s="69"/>
+      <c r="E536" s="70"/>
+      <c r="F536" s="69"/>
+      <c r="H536" s="9"/>
+      <c r="I536" s="71"/>
+      <c r="J536" s="71"/>
+      <c r="K536" s="71"/>
+      <c r="L536" s="72"/>
+      <c r="M536" s="72"/>
+    </row>
     <row r="537" spans="1:13" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="538" spans="1:13" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="539" spans="1:13" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -14158,6 +14493,8 @@
     <row r="4757" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="4758" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="4759" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="4760" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="4761" s="73" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A11:M12">
     <filterColumn colId="8" showButton="0"/>

</xml_diff>

<commit_message>
Agregados otros 3 casos de prueba
</commit_message>
<xml_diff>
--- a/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-4.xlsx
+++ b/docs/especificaciones/casos-de-prueba/Casos-de-Prueba-Parte-4.xlsx
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="99">
   <si>
     <t xml:space="preserve">RESULTADO OBTENIDO </t>
   </si>
@@ -358,6 +358,120 @@
   </si>
   <si>
     <t>Agendar en un día domingo</t>
+  </si>
+  <si>
+    <t>CUS-14 y CUS-26</t>
+  </si>
+  <si>
+    <t>Anular atención</t>
+  </si>
+  <si>
+    <t>Cancela una atención agendada</t>
+  </si>
+  <si>
+    <t>Anular atención normal</t>
+  </si>
+  <si>
+    <t>Anular atención pagada</t>
+  </si>
+  <si>
+    <t>Buscar paciente y anular atención agendada</t>
+  </si>
+  <si>
+    <t>Buscar paciente y anular atención pagada</t>
+  </si>
+  <si>
+    <t>Atención anulada</t>
+  </si>
+  <si>
+    <t>Atención anulada y con devolución de dinero</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de anulación</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de anulación y de devuelve el dinero</t>
+  </si>
+  <si>
+    <t>Se muestra un mensaje de error y no permite la anulación</t>
+  </si>
+  <si>
+    <t>CUS-3</t>
+  </si>
+  <si>
+    <t>Crear paciente</t>
+  </si>
+  <si>
+    <t>Crear un paciente en el sistema</t>
+  </si>
+  <si>
+    <t>Paciente ingresado correctamente</t>
+  </si>
+  <si>
+    <t>Ingresar paciente correcto</t>
+  </si>
+  <si>
+    <t>Ingresar paciente ya ingresado</t>
+  </si>
+  <si>
+    <t>Ingresar sin todos los datos</t>
+  </si>
+  <si>
+    <t>Llenar todos los campos correctamente</t>
+  </si>
+  <si>
+    <t>Llenar todos los campos correctamente y el Rut de un paciente ya ingresado</t>
+  </si>
+  <si>
+    <t>Dejar algunos campos en blanco</t>
+  </si>
+  <si>
+    <t>Paciente no se puede ingresar</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de creación correcta</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de que no se pudo crear el paciente</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de que el paciente ya está ingresado</t>
+  </si>
+  <si>
+    <t>CUS-6 y CUS-8</t>
+  </si>
+  <si>
+    <t>Ingresar paciente</t>
+  </si>
+  <si>
+    <t>Ingresa un paciente para su atención</t>
+  </si>
+  <si>
+    <t>Ingreso correcto</t>
+  </si>
+  <si>
+    <t>Paciente no tiene atenciones</t>
+  </si>
+  <si>
+    <t>Buscar paciente con una atención agendada e ingresarlo</t>
+  </si>
+  <si>
+    <t>Buscar paciente sin atenciones agendada</t>
+  </si>
+  <si>
+    <t>Paciente registrado correctamente</t>
+  </si>
+  <si>
+    <t>Paciente no tiene atenciones agendadas</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de ingreso correcto</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de que el paciente no existe</t>
+  </si>
+  <si>
+    <t>No hay atenciones en la lista de atenciones</t>
   </si>
 </sst>
 </file>
@@ -944,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1244,35 +1358,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1317,100 +1404,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1455,6 +1448,110 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="14" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1492,7 +1589,7 @@
         <xdr:cNvPr id="15407" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5116346C-80FE-4822-AA22-AB1007555EEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5116346C-80FE-4822-AA22-AB1007555EEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1663,7 @@
         <xdr:cNvPr id="15408" name="2 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20492279-609F-4EF7-B274-92F5096225C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20492279-609F-4EF7-B274-92F5096225C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1999,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="10.5" x14ac:dyDescent="0.2"/>
@@ -2035,35 +2132,35 @@
     </row>
     <row r="2" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
@@ -2075,21 +2172,21 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C5" s="102" t="s">
+      <c r="C5" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="102" t="s">
+      <c r="D5" s="130"/>
+      <c r="E5" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="105"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="129"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
@@ -2101,14 +2198,14 @@
       <c r="E6" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="110"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="109"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
@@ -2120,14 +2217,14 @@
       <c r="E7" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="109"/>
     </row>
     <row r="8" spans="1:15" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" s="106" t="s">
@@ -2137,87 +2234,87 @@
       <c r="E8" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="110"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="109"/>
     </row>
     <row r="9" spans="1:15" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="120" t="s">
+      <c r="C9" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="121"/>
-      <c r="E9" s="99">
+      <c r="D9" s="115"/>
+      <c r="E9" s="124">
         <v>42702</v>
       </c>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="117"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="111"/>
     </row>
     <row r="10" spans="1:15" s="8" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="113"/>
     </row>
     <row r="11" spans="1:15" s="10" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="114" t="s">
+      <c r="A11" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="126" t="s">
+      <c r="E11" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="114" t="s">
+      <c r="F11" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="114" t="s">
+      <c r="G11" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="114" t="s">
+      <c r="H11" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="123" t="s">
+      <c r="I11" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="125"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="119"/>
     </row>
     <row r="12" spans="1:15" s="10" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="115"/>
-      <c r="B12" s="115"/>
-      <c r="C12" s="129"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
       <c r="I12" s="11" t="s">
         <v>2</v>
       </c>
@@ -2235,7 +2332,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="81" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -2244,7 +2341,7 @@
       <c r="C13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="82" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="14" t="s">
@@ -2253,24 +2350,24 @@
       <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="90" t="s">
+      <c r="G13" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="89" t="s">
+      <c r="H13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="130" t="s">
+      <c r="I13" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="131"/>
-      <c r="M13" s="132" t="s">
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="94" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="81" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -2279,33 +2376,33 @@
       <c r="C14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="91" t="s">
+      <c r="D14" s="84" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="139" t="s">
+      <c r="F14" s="101" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="91" t="s">
+      <c r="H14" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="135" t="s">
+      <c r="I14" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
       <c r="L14" s="33"/>
       <c r="M14" s="36" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="81" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -2314,97 +2411,97 @@
       <c r="C15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="84" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="139" t="s">
+      <c r="F15" s="101" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="91" t="s">
+      <c r="H15" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="135" t="s">
+      <c r="I15" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="135"/>
-      <c r="K15" s="135"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
       <c r="L15" s="33"/>
       <c r="M15" s="36" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="133" t="s">
+      <c r="D16" s="95" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="140" t="s">
+      <c r="F16" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="134" t="s">
+      <c r="G16" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="133" t="s">
+      <c r="H16" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="136" t="s">
+      <c r="I16" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="136"/>
-      <c r="K16" s="136"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="138" t="s">
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="100" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="88" t="s">
+      <c r="B17" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="133" t="s">
+      <c r="D17" s="95" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="140" t="s">
+      <c r="F17" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="134" t="s">
+      <c r="G17" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="133" t="s">
+      <c r="H17" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="136" t="s">
+      <c r="I17" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="137"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="99"/>
       <c r="M17" s="36" t="s">
         <v>51</v>
       </c>
@@ -2416,10 +2513,10 @@
       <c r="B18" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="91" t="s">
+      <c r="D18" s="84" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="19" t="s">
@@ -2428,17 +2525,17 @@
       <c r="F18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="91" t="s">
+      <c r="G18" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="96" t="s">
+      <c r="H18" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="136" t="s">
+      <c r="I18" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="135"/>
-      <c r="K18" s="135"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
       <c r="L18" s="34"/>
       <c r="M18" s="36" t="s">
         <v>56</v>
@@ -2451,30 +2548,30 @@
       <c r="B19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="91" t="s">
+      <c r="D19" s="84" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="93" t="s">
+      <c r="G19" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="94" t="s">
+      <c r="H19" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="136" t="s">
+      <c r="I19" s="98" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
-      <c r="L19" s="92"/>
+      <c r="L19" s="85"/>
       <c r="M19" s="36" t="s">
         <v>57</v>
       </c>
@@ -2486,30 +2583,30 @@
       <c r="B20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="91" t="s">
+      <c r="D20" s="84" t="s">
         <v>42</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="95" t="s">
+      <c r="F20" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="93" t="s">
+      <c r="G20" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="96" t="s">
+      <c r="H20" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="136" t="s">
+      <c r="I20" s="98" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
-      <c r="L20" s="92"/>
+      <c r="L20" s="85"/>
       <c r="M20" s="36" t="s">
         <v>57</v>
       </c>
@@ -2521,168 +2618,348 @@
       <c r="B21" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="91" t="s">
+      <c r="D21" s="84" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="88" t="s">
+      <c r="G21" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="96" t="s">
+      <c r="H21" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="136" t="s">
+      <c r="I21" s="98" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="98"/>
+      <c r="L21" s="91"/>
       <c r="M21" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="135"/>
+    <row r="22" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="97" t="s">
+        <v>22</v>
+      </c>
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
-      <c r="L22" s="98"/>
-      <c r="M22" s="36"/>
-    </row>
-    <row r="23" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="35"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="89" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="38"/>
-    </row>
-    <row r="24" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="96"/>
-      <c r="I24" s="35"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
-      <c r="L24" s="98"/>
-      <c r="M24" s="36"/>
-    </row>
-    <row r="25" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="26"/>
-    </row>
-    <row r="26" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="23"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="90" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="134" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="24"/>
-    </row>
-    <row r="27" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
+      <c r="M26" s="38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J27" s="23"/>
       <c r="K27" s="23"/>
       <c r="L27" s="22"/>
-      <c r="M27" s="24"/>
-    </row>
-    <row r="28" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="26"/>
-    </row>
-    <row r="29" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
+      <c r="M27" s="38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="15" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="134" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="136" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
       <c r="L29" s="22"/>
-      <c r="M29" s="24"/>
-    </row>
-    <row r="30" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
+      <c r="M29" s="38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="15" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="136" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="134" t="s">
+        <v>22</v>
+      </c>
       <c r="J30" s="23"/>
       <c r="K30" s="23"/>
       <c r="L30" s="22"/>
-      <c r="M30" s="24"/>
+      <c r="M30" s="38" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31" spans="1:13" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
@@ -14503,6 +14780,17 @@
     <filterColumn colId="11" showButton="0"/>
   </autoFilter>
   <mergeCells count="27">
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="D3:K3"/>
@@ -14519,17 +14807,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>